<commit_message>
Update preprocess and calibration data
</commit_message>
<xml_diff>
--- a/calibration_log.xlsx
+++ b/calibration_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hungyunlu/Library/CloudStorage/Box-Box/Hung-Yun Lu Research File/Projects/FSCV/EN_FSCV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01350D7-2519-644F-B71B-764BA05EE0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC4F9E0-A41B-0C4D-A241-F36811F8C127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{70EFF65A-D3A6-CC4B-ADFE-BB01482CA67A}"/>
   </bookViews>
@@ -555,7 +555,7 @@
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>

</xml_diff>